<commit_message>
Added the code for Setting the batch definition; Event and Alerts page
</commit_message>
<xml_diff>
--- a/src/main/resources/config/automation2/TestData/UploadFile.xlsx
+++ b/src/main/resources/config/automation2/TestData/UploadFile.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="43">
   <si>
     <t>CER_SEQUENCE</t>
   </si>
@@ -154,9 +154,6 @@
   </si>
   <si>
     <t>CORPORATE TRAVEL CARD SINGLE CURRENCY [P00006]</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
 </sst>
 </file>
@@ -588,9 +585,7 @@
       <c r="H2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>43</v>
-      </c>
+      <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="1"/>
     </row>
@@ -619,9 +614,7 @@
       <c r="H3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>43</v>
-      </c>
+      <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="1"/>
     </row>
@@ -650,9 +643,7 @@
       <c r="H4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>43</v>
-      </c>
+      <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="1"/>
     </row>
@@ -681,9 +672,7 @@
       <c r="H5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>43</v>
-      </c>
+      <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="1"/>
     </row>

</xml_diff>